<commit_message>
inclusao do SIPOC do projeto
</commit_message>
<xml_diff>
--- a/causa-raiz/Plano_de_acao.xlsx
+++ b/causa-raiz/Plano_de_acao.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\rh_turnover_dmaic_causa_raiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\rh_turnover_dmaic_causa_raiz\causa-raiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4B67F50-A22A-42C8-B7ED-6225861F909B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F35C17-7C14-4333-943D-895844FABEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70E88DC1-8289-4571-90BA-25D3263E3938}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="5W2H" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1322,7 +1322,7 @@
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>